<commit_message>
Add merge without m3u8
</commit_message>
<xml_diff>
--- a/evaData/eva.xlsx
+++ b/evaData/eva.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\go\Distributed-meeting-recording-storage\evaData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABC8834-C8FA-4077-88EF-1ED4F0002DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3386B389-D91D-4864-AFE4-803150B9D4B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9560" yWindow="3080" windowWidth="22000" windowHeight="14670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6550" yWindow="6590" windowWidth="22000" windowHeight="14670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
   <si>
     <t>4k</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -78,15 +78,162 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>merge1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>merge2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>merge3</t>
+    <t>Merge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3worker</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8worker</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10worker</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Process Time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Worker</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3Worker</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8Worker</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2Requester</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12Requertser</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12Worker</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8Requester</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Server</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>360 Convert</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>360 Merge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1080 Convert</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1080 Merge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4k Convert</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4K Merge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1080 Tramission Time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>360 Tramission Time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4K Tramission Time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.61,2.71;1.38,2.16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>141.12,133.12;120.22,120.53</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.61,2.71;1.38,2.17</t>
+  </si>
+  <si>
+    <t>1.61,2.71;1.38,2.18</t>
+  </si>
+  <si>
+    <t>32.71,23.16;22.64,30.29</t>
+  </si>
+  <si>
+    <t>32.71,23.16;22.64,30.30</t>
+  </si>
+  <si>
+    <t>141.12,133.12;120.22,120.54</t>
+  </si>
+  <si>
+    <t>141.12,133.12;120.22,120.55</t>
+  </si>
+  <si>
+    <t>32.71,23.16;22.64,30.28;22.90,30.68</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>new_360</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MergeSpeed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>40.9,43.37</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>new_1080</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>194.22,183.26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>new_4k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4 to 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 to 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -129,10 +276,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -414,16 +568,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.4140625" customWidth="1"/>
     <col min="3" max="3" width="12.9140625" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -438,14 +593,14 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4">
@@ -495,6 +650,20 @@
         <v>192.4</v>
       </c>
     </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <f>AVERAGE(B6:B8)</f>
+        <v>5.9899999999999993</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:D9" si="0">AVERAGE(C6:C8)</f>
+        <v>40.903333333333336</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>192.24</v>
+      </c>
+    </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1</v>
@@ -546,10 +715,293 @@
         <v>12</v>
       </c>
     </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" t="s">
+        <v>43</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="2">
+        <v>5.99</v>
+      </c>
+      <c r="I21" s="4">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>7.8</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="I22" s="4">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31">
+        <f>3.04+3.04</f>
+        <v>6.08</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32">
+        <f>6.1</f>
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33">
+        <f>3.02+12*3.02/5.12</f>
+        <v>10.098125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>42</v>
+      </c>
+      <c r="B49">
+        <v>2.65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>46</v>
+      </c>
+      <c r="B50">
+        <v>68.599999999999994</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>48</v>
+      </c>
+      <c r="B51">
+        <v>149</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="8">
+    <mergeCell ref="N29:O29"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="F3:H3"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:M29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>